<commit_message>
Updated employment targets inline with the new initial populations
</commit_message>
<xml_diff>
--- a/input/PL/employment_targets.xlsx
+++ b/input/PL/employment_targets.xlsx
@@ -87,7 +87,7 @@
         <v>2011</v>
       </c>
       <c r="B2">
-        <v>0.82383029192035362</v>
+        <v>0.81926267736065861</v>
       </c>
     </row>
     <row r="3">
@@ -95,7 +95,7 @@
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.821731322462114</v>
+        <v>0.81816541766195372</v>
       </c>
     </row>
     <row r="4">
@@ -103,7 +103,7 @@
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.81609950788251906</v>
+        <v>0.81263969347138987</v>
       </c>
     </row>
     <row r="5">
@@ -111,7 +111,7 @@
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.83106676793864132</v>
+        <v>0.82765408852075384</v>
       </c>
     </row>
     <row r="6">
@@ -119,7 +119,7 @@
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.83335242550016386</v>
+        <v>0.82950872081543936</v>
       </c>
     </row>
     <row r="7">
@@ -127,7 +127,7 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.83973543797809402</v>
+        <v>0.83611248688842976</v>
       </c>
     </row>
     <row r="8">
@@ -135,7 +135,7 @@
         <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.84157973500650807</v>
+        <v>0.83775723517092482</v>
       </c>
     </row>
     <row r="9">
@@ -143,7 +143,7 @@
         <v>2018</v>
       </c>
       <c r="B9">
-        <v>0.84545298666168944</v>
+        <v>0.84284125820157529</v>
       </c>
     </row>
     <row r="10">
@@ -151,7 +151,7 @@
         <v>2019</v>
       </c>
       <c r="B10">
-        <v>0.8534134938695962</v>
+        <v>0.84858463562677389</v>
       </c>
     </row>
     <row r="11">
@@ -159,7 +159,7 @@
         <v>2020</v>
       </c>
       <c r="B11">
-        <v>0.86500591632281076</v>
+        <v>0.86186749844364374</v>
       </c>
     </row>
     <row r="12">
@@ -167,7 +167,7 @@
         <v>2021</v>
       </c>
       <c r="B12">
-        <v>0.88091732038400394</v>
+        <v>0.8771080374304252</v>
       </c>
     </row>
     <row r="13">
@@ -175,7 +175,7 @@
         <v>2022</v>
       </c>
       <c r="B13">
-        <v>0.87862197711765877</v>
+        <v>0.87584419058033092</v>
       </c>
     </row>
     <row r="14">
@@ -183,7 +183,7 @@
         <v>2023</v>
       </c>
       <c r="B14">
-        <v>0.89231035103286582</v>
+        <v>0.88957720844980337</v>
       </c>
     </row>
   </sheetData>
@@ -211,7 +211,7 @@
         <v>2011</v>
       </c>
       <c r="B2">
-        <v>0.38052187841351931</v>
+        <v>0.3991450072596518</v>
       </c>
     </row>
     <row r="3">
@@ -219,7 +219,7 @@
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.39494946229994121</v>
+        <v>0.41948999821695471</v>
       </c>
     </row>
     <row r="4">
@@ -227,7 +227,7 @@
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.3708155540743337</v>
+        <v>0.39157863662299497</v>
       </c>
     </row>
     <row r="5">
@@ -235,7 +235,7 @@
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.39400614231074099</v>
+        <v>0.41433692743405076</v>
       </c>
     </row>
     <row r="6">
@@ -243,7 +243,7 @@
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.39038070193201418</v>
+        <v>0.41124963262829567</v>
       </c>
     </row>
     <row r="7">
@@ -251,7 +251,7 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.4045626857325601</v>
+        <v>0.42607921647394814</v>
       </c>
     </row>
     <row r="8">
@@ -259,7 +259,7 @@
         <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.43452589116520407</v>
+        <v>0.45788102982282675</v>
       </c>
     </row>
     <row r="9">
@@ -267,7 +267,7 @@
         <v>2018</v>
       </c>
       <c r="B9">
-        <v>0.41769307045724119</v>
+        <v>0.43475036545320306</v>
       </c>
     </row>
     <row r="10">
@@ -275,7 +275,7 @@
         <v>2019</v>
       </c>
       <c r="B10">
-        <v>0.42367705016359092</v>
+        <v>0.4352103131468209</v>
       </c>
     </row>
     <row r="11">
@@ -283,7 +283,7 @@
         <v>2020</v>
       </c>
       <c r="B11">
-        <v>0.45367977278524363</v>
+        <v>0.48020557694901034</v>
       </c>
     </row>
     <row r="12">
@@ -291,7 +291,7 @@
         <v>2021</v>
       </c>
       <c r="B12">
-        <v>0.44799750636445951</v>
+        <v>0.45212571734411705</v>
       </c>
     </row>
     <row r="13">
@@ -299,7 +299,7 @@
         <v>2022</v>
       </c>
       <c r="B13">
-        <v>0.43338321233616106</v>
+        <v>0.43647713649597536</v>
       </c>
     </row>
     <row r="14">
@@ -307,7 +307,7 @@
         <v>2023</v>
       </c>
       <c r="B14">
-        <v>0.43184882342437486</v>
+        <v>0.43758876928331342</v>
       </c>
     </row>
   </sheetData>
@@ -335,7 +335,7 @@
         <v>2011</v>
       </c>
       <c r="B2">
-        <v>0.51193623756613316</v>
+        <v>0.53742812155347619</v>
       </c>
     </row>
     <row r="3">
@@ -343,7 +343,7 @@
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.51388796407993187</v>
+        <v>0.53844044474943309</v>
       </c>
     </row>
     <row r="4">
@@ -351,7 +351,7 @@
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.50731054213776516</v>
+        <v>0.52988290374081737</v>
       </c>
     </row>
     <row r="5">
@@ -359,7 +359,7 @@
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.51131531460632029</v>
+        <v>0.54149128104056998</v>
       </c>
     </row>
     <row r="6">
@@ -367,7 +367,7 @@
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.53318545452592403</v>
+        <v>0.55716858320426854</v>
       </c>
     </row>
     <row r="7">
@@ -375,7 +375,7 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.58285048457054911</v>
+        <v>0.6085817810490497</v>
       </c>
     </row>
     <row r="8">
@@ -383,7 +383,7 @@
         <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.59181134292156978</v>
+        <v>0.61658657335201739</v>
       </c>
     </row>
     <row r="9">
@@ -391,7 +391,7 @@
         <v>2018</v>
       </c>
       <c r="B9">
-        <v>0.56828787809135639</v>
+        <v>0.59176278878693189</v>
       </c>
     </row>
     <row r="10">
@@ -399,7 +399,7 @@
         <v>2019</v>
       </c>
       <c r="B10">
-        <v>0.57210350926861453</v>
+        <v>0.58548745841077365</v>
       </c>
     </row>
     <row r="11">
@@ -407,7 +407,7 @@
         <v>2020</v>
       </c>
       <c r="B11">
-        <v>0.56859266378921847</v>
+        <v>0.58854728020588165</v>
       </c>
     </row>
     <row r="12">
@@ -415,7 +415,7 @@
         <v>2021</v>
       </c>
       <c r="B12">
-        <v>0.61407456424300411</v>
+        <v>0.62663450587764535</v>
       </c>
     </row>
     <row r="13">
@@ -423,7 +423,7 @@
         <v>2022</v>
       </c>
       <c r="B13">
-        <v>0.60188645030954646</v>
+        <v>0.61267069061990309</v>
       </c>
     </row>
     <row r="14">
@@ -431,7 +431,7 @@
         <v>2023</v>
       </c>
       <c r="B14">
-        <v>0.59164974063354814</v>
+        <v>0.6023965824847306</v>
       </c>
     </row>
   </sheetData>
@@ -459,7 +459,7 @@
         <v>2011</v>
       </c>
       <c r="B2">
-        <v>0.30785190812656721</v>
+        <v>0.30960911864445839</v>
       </c>
     </row>
     <row r="3">
@@ -467,7 +467,7 @@
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.30811218783286087</v>
+        <v>0.3009604726704741</v>
       </c>
     </row>
     <row r="4">
@@ -475,7 +475,7 @@
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.31195865499437081</v>
+        <v>0.30537970485383314</v>
       </c>
     </row>
     <row r="5">
@@ -483,7 +483,7 @@
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.28581726919907879</v>
+        <v>0.27890116565669643</v>
       </c>
     </row>
     <row r="6">
@@ -491,7 +491,7 @@
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.27963714773111775</v>
+        <v>0.27448488810723043</v>
       </c>
     </row>
     <row r="7">
@@ -499,7 +499,7 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.30752858106411018</v>
+        <v>0.30109497280240638</v>
       </c>
     </row>
     <row r="8">
@@ -507,7 +507,7 @@
         <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.30346469681990601</v>
+        <v>0.30056498819528676</v>
       </c>
     </row>
     <row r="9">
@@ -515,7 +515,7 @@
         <v>2018</v>
       </c>
       <c r="B9">
-        <v>0.31364752176359245</v>
+        <v>0.30681190730380958</v>
       </c>
     </row>
     <row r="10">
@@ -523,7 +523,7 @@
         <v>2019</v>
       </c>
       <c r="B10">
-        <v>0.35381764642659308</v>
+        <v>0.35913699591968529</v>
       </c>
     </row>
     <row r="11">
@@ -531,7 +531,7 @@
         <v>2020</v>
       </c>
       <c r="B11">
-        <v>0.34820741422940238</v>
+        <v>0.34448547398830465</v>
       </c>
     </row>
     <row r="12">
@@ -539,7 +539,7 @@
         <v>2021</v>
       </c>
       <c r="B12">
-        <v>0.3607173104243539</v>
+        <v>0.35897695098347643</v>
       </c>
     </row>
     <row r="13">
@@ -547,7 +547,7 @@
         <v>2022</v>
       </c>
       <c r="B13">
-        <v>0.36274965739361886</v>
+        <v>0.3588495010998119</v>
       </c>
     </row>
     <row r="14">
@@ -555,7 +555,7 @@
         <v>2023</v>
       </c>
       <c r="B14">
-        <v>0.36845418733118185</v>
+        <v>0.36154285650172741</v>
       </c>
     </row>
   </sheetData>
@@ -583,7 +583,7 @@
         <v>2011</v>
       </c>
       <c r="B2">
-        <v>0.41894661081369583</v>
+        <v>0.41638526322582725</v>
       </c>
     </row>
     <row r="3">
@@ -591,7 +591,7 @@
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.40321361657827082</v>
+        <v>0.4000992497086247</v>
       </c>
     </row>
     <row r="4">
@@ -599,7 +599,7 @@
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.39961607117918457</v>
+        <v>0.39148649281255121</v>
       </c>
     </row>
     <row r="5">
@@ -607,7 +607,7 @@
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.39812522211769624</v>
+        <v>0.39413842587482062</v>
       </c>
     </row>
     <row r="6">
@@ -615,7 +615,7 @@
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.40991729842040864</v>
+        <v>0.40679199236816832</v>
       </c>
     </row>
     <row r="7">
@@ -623,7 +623,7 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.40545695127308695</v>
+        <v>0.40240254301445588</v>
       </c>
     </row>
     <row r="8">
@@ -631,7 +631,7 @@
         <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.41228362735812552</v>
+        <v>0.41093893006058185</v>
       </c>
     </row>
     <row r="9">
@@ -639,7 +639,7 @@
         <v>2018</v>
       </c>
       <c r="B9">
-        <v>0.42686713226978734</v>
+        <v>0.42075425802135913</v>
       </c>
     </row>
     <row r="10">
@@ -647,7 +647,7 @@
         <v>2019</v>
       </c>
       <c r="B10">
-        <v>0.42517186848982991</v>
+        <v>0.42573444595703996</v>
       </c>
     </row>
     <row r="11">
@@ -655,7 +655,7 @@
         <v>2020</v>
       </c>
       <c r="B11">
-        <v>0.41013480515252171</v>
+        <v>0.40895011068374643</v>
       </c>
     </row>
     <row r="12">
@@ -663,7 +663,7 @@
         <v>2021</v>
       </c>
       <c r="B12">
-        <v>0.43258856779953725</v>
+        <v>0.43199059291587072</v>
       </c>
     </row>
     <row r="13">
@@ -671,7 +671,7 @@
         <v>2022</v>
       </c>
       <c r="B13">
-        <v>0.44326586886465918</v>
+        <v>0.43794253919446102</v>
       </c>
     </row>
     <row r="14">
@@ -679,7 +679,7 @@
         <v>2023</v>
       </c>
       <c r="B14">
-        <v>0.46207239052048033</v>
+        <v>0.45836433725671061</v>
       </c>
     </row>
   </sheetData>
@@ -707,7 +707,7 @@
         <v>2011</v>
       </c>
       <c r="B2">
-        <v>0.30208181732795336</v>
+        <v>0.29890599073681112</v>
       </c>
     </row>
     <row r="3">
@@ -715,7 +715,7 @@
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.30061108532233771</v>
+        <v>0.30143439406655592</v>
       </c>
     </row>
     <row r="4">
@@ -723,7 +723,7 @@
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.30276407721188736</v>
+        <v>0.30152689696624108</v>
       </c>
     </row>
     <row r="5">
@@ -731,7 +731,7 @@
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.31145040929785739</v>
+        <v>0.31000832388467597</v>
       </c>
     </row>
     <row r="6">
@@ -739,7 +739,7 @@
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.31244190895581908</v>
+        <v>0.30977756771418391</v>
       </c>
     </row>
     <row r="7">
@@ -747,7 +747,7 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.31288817157553944</v>
+        <v>0.31115539905180917</v>
       </c>
     </row>
     <row r="8">
@@ -755,7 +755,7 @@
         <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.30967743686400945</v>
+        <v>0.30826073273200044</v>
       </c>
     </row>
     <row r="9">
@@ -763,7 +763,7 @@
         <v>2018</v>
       </c>
       <c r="B9">
-        <v>0.3052372997493929</v>
+        <v>0.30027367523619586</v>
       </c>
     </row>
     <row r="10">
@@ -771,7 +771,7 @@
         <v>2019</v>
       </c>
       <c r="B10">
-        <v>0.31519769527800484</v>
+        <v>0.3114533855079103</v>
       </c>
     </row>
     <row r="11">
@@ -779,7 +779,7 @@
         <v>2020</v>
       </c>
       <c r="B11">
-        <v>0.31410432759222856</v>
+        <v>0.31075908202123842</v>
       </c>
     </row>
     <row r="12">
@@ -787,7 +787,7 @@
         <v>2021</v>
       </c>
       <c r="B12">
-        <v>0.319650585035544</v>
+        <v>0.31838468917312085</v>
       </c>
     </row>
     <row r="13">
@@ -795,7 +795,7 @@
         <v>2022</v>
       </c>
       <c r="B13">
-        <v>0.34466439690323852</v>
+        <v>0.34228404069903945</v>
       </c>
     </row>
     <row r="14">
@@ -803,7 +803,7 @@
         <v>2023</v>
       </c>
       <c r="B14">
-        <v>0.34069381864858117</v>
+        <v>0.33890969837670926</v>
       </c>
     </row>
   </sheetData>
@@ -831,7 +831,7 @@
         <v>2011</v>
       </c>
       <c r="B2">
-        <v>0.44580390908196338</v>
+        <v>0.44718650879882615</v>
       </c>
     </row>
     <row r="3">
@@ -839,7 +839,7 @@
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.44324938187318652</v>
+        <v>0.44121448255095902</v>
       </c>
     </row>
     <row r="4">
@@ -847,7 +847,7 @@
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.44437298985301549</v>
+        <v>0.44471308403527815</v>
       </c>
     </row>
     <row r="5">
@@ -855,7 +855,7 @@
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.45665144279125908</v>
+        <v>0.4533156680533294</v>
       </c>
     </row>
     <row r="6">
@@ -863,7 +863,7 @@
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.47060122836212664</v>
+        <v>0.47460676585552064</v>
       </c>
     </row>
     <row r="7">
@@ -871,7 +871,7 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.46283571902209464</v>
+        <v>0.46812326004996629</v>
       </c>
     </row>
     <row r="8">
@@ -879,7 +879,7 @@
         <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.4829455027595948</v>
+        <v>0.48024505747805785</v>
       </c>
     </row>
     <row r="9">
@@ -887,7 +887,7 @@
         <v>2018</v>
       </c>
       <c r="B9">
-        <v>0.49083580436737168</v>
+        <v>0.48649978080337819</v>
       </c>
     </row>
     <row r="10">
@@ -895,7 +895,7 @@
         <v>2019</v>
       </c>
       <c r="B10">
-        <v>0.48680351073667416</v>
+        <v>0.48701374677103965</v>
       </c>
     </row>
     <row r="11">
@@ -903,7 +903,7 @@
         <v>2020</v>
       </c>
       <c r="B11">
-        <v>0.49651737484706926</v>
+        <v>0.49963984755210444</v>
       </c>
     </row>
     <row r="12">
@@ -911,7 +911,7 @@
         <v>2021</v>
       </c>
       <c r="B12">
-        <v>0.52320974701450895</v>
+        <v>0.52688230019279025</v>
       </c>
     </row>
     <row r="13">
@@ -919,7 +919,7 @@
         <v>2022</v>
       </c>
       <c r="B13">
-        <v>0.53678039526990218</v>
+        <v>0.53298706390936279</v>
       </c>
     </row>
     <row r="14">
@@ -927,7 +927,7 @@
         <v>2023</v>
       </c>
       <c r="B14">
-        <v>0.52108578146447826</v>
+        <v>0.51857282738817789</v>
       </c>
     </row>
   </sheetData>

</xml_diff>